<commit_message>
Integrated 2023 and fixed many issues
</commit_message>
<xml_diff>
--- a/database/PLM/PLM2023.xlsx
+++ b/database/PLM/PLM2023.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0-my.sharepoint.com/personal/christophe_danjou_polymtl_ca/Documents/Bureau/PLM23/Liste_soumission/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyfelix/dev/plmstudy/database/PLM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E06E030-55A3-4190-B015-28859892C621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3BEB5DE-DDF5-E547-B601-E5E9DBFFC5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="papers" sheetId="1" r:id="rId1"/>
+    <sheet name="PLM2023" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">papers!$A$1:$D$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PLM2023'!$A$1:$D$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -701,9 +701,6 @@
     <t>An Implementation of Integrated Approach in Product Life-cycle Management Tool to Ensure Requirements-In-Loop during Complex Product Development: A Cubesat Case Study</t>
   </si>
   <si>
-    <t>Model Based Systems Engineering · RFLP · Requirements- in-Loop· Product Life-cycle Management · Decision Support</t>
-  </si>
-  <si>
     <t>Oliva, Manuel (1);
 Arista, Rebeca (2,3);
 Morales-Palma, Domingo (3);
@@ -766,13 +763,16 @@
     <t>Hybrid Production Structures as a Solution for Flexibility and Transformability for Longer Life Cycles of Production Systems</t>
   </si>
   <si>
-    <t>Hybrid Production Structures; Flow Production; Job Shop Production; Flexibility; Interdependencies; Transformability; Life Cycle</t>
+    <t>Model Based Systems Engineering, RFLP, Requirements- in-Loop, Product Life-cycle Management,Decision Support</t>
+  </si>
+  <si>
+    <t>Hybrid Production Structures, Flow Production, Job Shop Production, Flexibility, Interdependencies, Transformability, Life Cycle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1256,53 +1256,56 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1318,7 +1321,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1613,22 +1616,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C41" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.20703125" customWidth="1"/>
-    <col min="2" max="2" width="9.83984375" customWidth="1"/>
-    <col min="3" max="3" width="125.734375" customWidth="1"/>
-    <col min="4" max="4" width="114.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="125.6640625" customWidth="1"/>
+    <col min="4" max="4" width="114.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1642,11 +1645,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C2" t="s">
@@ -1656,7 +1659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1684,7 +1687,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1712,7 +1715,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1754,7 +1757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1768,7 +1771,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1796,7 +1799,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1810,7 +1813,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1880,7 +1883,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1922,7 +1925,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1936,7 +1939,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>25</v>
       </c>
@@ -1978,7 +1981,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1992,7 +1995,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>27</v>
       </c>
@@ -2006,7 +2009,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>28</v>
       </c>
@@ -2020,7 +2023,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>29</v>
       </c>
@@ -2034,7 +2037,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>30</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>31</v>
       </c>
@@ -2062,7 +2065,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>32</v>
       </c>
@@ -2076,7 +2079,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>33</v>
       </c>
@@ -2090,7 +2093,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
@@ -2104,7 +2107,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>35</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>36</v>
       </c>
@@ -2132,7 +2135,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>37</v>
       </c>
@@ -2146,7 +2149,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>38</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>39</v>
       </c>
@@ -2174,7 +2177,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
@@ -2188,7 +2191,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>41</v>
       </c>
@@ -2202,7 +2205,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>42</v>
       </c>
@@ -2216,7 +2219,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>43</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>44</v>
       </c>
@@ -2244,7 +2247,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2258,7 +2261,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>46</v>
       </c>
@@ -2272,7 +2275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>47</v>
       </c>
@@ -2286,7 +2289,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>48</v>
       </c>
@@ -2300,7 +2303,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2314,7 +2317,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2328,7 +2331,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>51</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>52</v>
       </c>
@@ -2356,7 +2359,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>53</v>
       </c>
@@ -2370,7 +2373,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>54</v>
       </c>
@@ -2384,7 +2387,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>55</v>
       </c>
@@ -2398,7 +2401,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>56</v>
       </c>
@@ -2409,43 +2412,43 @@
         <v>170</v>
       </c>
       <c r="D56" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>57</v>
       </c>
       <c r="B57" t="s">
+        <v>171</v>
+      </c>
+      <c r="C57" t="s">
         <v>172</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>173</v>
       </c>
-      <c r="D57" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>58</v>
       </c>
       <c r="B58" t="s">
+        <v>174</v>
+      </c>
+      <c r="C58" t="s">
         <v>175</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>176</v>
       </c>
-      <c r="D58" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C59" t="s">
         <v>47</v>
@@ -2454,50 +2457,50 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>60</v>
       </c>
       <c r="B60" t="s">
+        <v>178</v>
+      </c>
+      <c r="C60" t="s">
         <v>179</v>
-      </c>
-      <c r="C60" t="s">
-        <v>180</v>
       </c>
       <c r="D60" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>61</v>
       </c>
       <c r="B61" t="s">
+        <v>180</v>
+      </c>
+      <c r="C61" t="s">
         <v>181</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>182</v>
       </c>
-      <c r="D61" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>62</v>
       </c>
       <c r="B62" t="s">
+        <v>183</v>
+      </c>
+      <c r="C62" t="s">
         <v>184</v>
-      </c>
-      <c r="C62" t="s">
-        <v>185</v>
       </c>
       <c r="D62" t="s">
         <v>186</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D62"/>
+  <autoFilter ref="A1:D62" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
 </worksheet>
 </file>
</xml_diff>